<commit_message>
dynamic feature excel sheet, training code, model, predict code but this idea wont work
</commit_message>
<xml_diff>
--- a/VisionModel/one_model/output/predicted_trajectoriesCombined.xlsx
+++ b/VisionModel/one_model/output/predicted_trajectoriesCombined.xlsx
@@ -460,13 +460,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>4042.261178533166</v>
+        <v>1571.110000049326</v>
       </c>
       <c r="C2" t="n">
-        <v>99.63138986942523</v>
+        <v>274.5400000030443</v>
       </c>
       <c r="D2" t="n">
-        <v>2872.758718594442</v>
+        <v>2788.830000029995</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>0.03333333333333333</v>
       </c>
       <c r="B3" t="n">
-        <v>4843.104700189625</v>
+        <v>2383.240000027599</v>
       </c>
       <c r="C3" t="n">
-        <v>133.684749483326</v>
+        <v>297.3199999984293</v>
       </c>
       <c r="D3" t="n">
-        <v>3335.020037985748</v>
+        <v>3318.210000016494</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>0.06666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>5694.049009783843</v>
+        <v>3167.01000002484</v>
       </c>
       <c r="C4" t="n">
-        <v>132.0249906400697</v>
+        <v>292.0400000030752</v>
       </c>
       <c r="D4" t="n">
-        <v>3798.162259809709</v>
+        <v>3856.950000006812</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>6438.611309263215</v>
+        <v>3929.380000025288</v>
       </c>
       <c r="C5" t="n">
-        <v>146.4752784414153</v>
+        <v>292.4500000063812</v>
       </c>
       <c r="D5" t="n">
-        <v>4245.31533836317</v>
+        <v>4345.590000004549</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="B6" t="n">
-        <v>7059.882565624657</v>
+        <v>4505.530000018184</v>
       </c>
       <c r="C6" t="n">
-        <v>163.6983367069226</v>
+        <v>311.4300000009518</v>
       </c>
       <c r="D6" t="n">
-        <v>4600.02708193398</v>
+        <v>4718.390000000028</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="B7" t="n">
-        <v>7603.291433288357</v>
+        <v>4997.76000001644</v>
       </c>
       <c r="C7" t="n">
-        <v>173.9658407765299</v>
+        <v>312.0700000017562</v>
       </c>
       <c r="D7" t="n">
-        <v>4833.91336467765</v>
+        <v>5030.869999999372</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>8032.262111407125</v>
+        <v>5410.030000016259</v>
       </c>
       <c r="C8" t="n">
-        <v>190.6088938661355</v>
+        <v>331.6100000020058</v>
       </c>
       <c r="D8" t="n">
-        <v>5058.054074345984</v>
+        <v>5275.739999995401</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>0.2333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>8313.879475221485</v>
+        <v>5845.5200000103</v>
       </c>
       <c r="C9" t="n">
-        <v>199.6609295146157</v>
+        <v>343.7600000025757</v>
       </c>
       <c r="D9" t="n">
-        <v>5296.037405313211</v>
+        <v>5553.899999997995</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="B10" t="n">
-        <v>8729.470243753516</v>
+        <v>6268.930000013829</v>
       </c>
       <c r="C10" t="n">
-        <v>212.6384564337307</v>
+        <v>347.7900000005106</v>
       </c>
       <c r="D10" t="n">
-        <v>5451.621370691195</v>
+        <v>5778.159999993276</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>0.3</v>
       </c>
       <c r="B11" t="n">
-        <v>9112.563602116979</v>
+        <v>6685.410000010121</v>
       </c>
       <c r="C11" t="n">
-        <v>238.6504178826896</v>
+        <v>354.2300000000048</v>
       </c>
       <c r="D11" t="n">
-        <v>5629.086028057161</v>
+        <v>6036.049999996207</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="B12" t="n">
-        <v>9453.505841529721</v>
+        <v>6968.70000000934</v>
       </c>
       <c r="C12" t="n">
-        <v>243.6519269973406</v>
+        <v>357.7699999983905</v>
       </c>
       <c r="D12" t="n">
-        <v>5764.157092739942</v>
+        <v>6182.399999994025</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>0.3666666666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>9774.924001650776</v>
+        <v>7315.880000013184</v>
       </c>
       <c r="C13" t="n">
-        <v>258.6806115824122</v>
+        <v>373.4699999995082</v>
       </c>
       <c r="D13" t="n">
-        <v>5898.040155849277</v>
+        <v>6337.779999992428</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +628,13 @@
         <v>0.4</v>
       </c>
       <c r="B14" t="n">
-        <v>10177.41970499595</v>
+        <v>7642.340000007943</v>
       </c>
       <c r="C14" t="n">
-        <v>277.3238092996165</v>
+        <v>385.2800000009273</v>
       </c>
       <c r="D14" t="n">
-        <v>6027.284754104194</v>
+        <v>6505.66999999364</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +642,13 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="B15" t="n">
-        <v>10457.61164861421</v>
+        <v>7942.840000003797</v>
       </c>
       <c r="C15" t="n">
-        <v>285.959734488659</v>
+        <v>395.6700000015693</v>
       </c>
       <c r="D15" t="n">
-        <v>6129.933177734317</v>
+        <v>6623.369999998818</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +656,13 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="B16" t="n">
-        <v>10739.56104438033</v>
+        <v>8211.29000000339</v>
       </c>
       <c r="C16" t="n">
-        <v>331.8596349857691</v>
+        <v>401.2499999987305</v>
       </c>
       <c r="D16" t="n">
-        <v>6242.907871355815</v>
+        <v>6731.089999994469</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +670,13 @@
         <v>0.5</v>
       </c>
       <c r="B17" t="n">
-        <v>10991.37258145039</v>
+        <v>8421.110000003007</v>
       </c>
       <c r="C17" t="n">
-        <v>341.3306269331836</v>
+        <v>412.3299999969155</v>
       </c>
       <c r="D17" t="n">
-        <v>6313.858401919963</v>
+        <v>6804.669999988783</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +684,13 @@
         <v>0.5333333333333333</v>
       </c>
       <c r="B18" t="n">
-        <v>11177.68563349658</v>
+        <v>8687.100000003398</v>
       </c>
       <c r="C18" t="n">
-        <v>347.8315910842927</v>
+        <v>413.3100000000913</v>
       </c>
       <c r="D18" t="n">
-        <v>6338.408447373296</v>
+        <v>6891.139999989607</v>
       </c>
     </row>
     <row r="19">
@@ -698,13 +698,13 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>11417.61049189586</v>
+        <v>8971.030000005254</v>
       </c>
       <c r="C19" t="n">
-        <v>367.4942650344049</v>
+        <v>439.259999998176</v>
       </c>
       <c r="D19" t="n">
-        <v>6366.887305438978</v>
+        <v>6975.359999986497</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +712,13 @@
         <v>0.6</v>
       </c>
       <c r="B20" t="n">
-        <v>11595.06932656615</v>
+        <v>9256.210000000277</v>
       </c>
       <c r="C20" t="n">
-        <v>381.6807619050949</v>
+        <v>457.7999999929814</v>
       </c>
       <c r="D20" t="n">
-        <v>6446.558841296247</v>
+        <v>7071.049999983691</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +726,13 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>11777.512002425</v>
+        <v>9430.740000004758</v>
       </c>
       <c r="C21" t="n">
-        <v>384.4399606484644</v>
+        <v>450.6400000024637</v>
       </c>
       <c r="D21" t="n">
-        <v>6463.165291660873</v>
+        <v>7093.659999957395</v>
       </c>
     </row>
     <row r="22">
@@ -740,13 +740,13 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>11997.33539222781</v>
+        <v>9565.119999998285</v>
       </c>
       <c r="C22" t="n">
-        <v>391.6039521416105</v>
+        <v>454.6500000005836</v>
       </c>
       <c r="D22" t="n">
-        <v>6489.928969743357</v>
+        <v>7081.369999981678</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>0.7</v>
       </c>
       <c r="B23" t="n">
-        <v>12128.77514305258</v>
+        <v>9660.709999993989</v>
       </c>
       <c r="C23" t="n">
-        <v>398.3599774891508</v>
+        <v>461.4300000003938</v>
       </c>
       <c r="D23" t="n">
-        <v>6449.104745751848</v>
+        <v>7030.679999993657</v>
       </c>
     </row>
     <row r="24">
@@ -768,13 +768,13 @@
         <v>0.7333333333333333</v>
       </c>
       <c r="B24" t="n">
-        <v>12392.78709634662</v>
+        <v>9942.999999999667</v>
       </c>
       <c r="C24" t="n">
-        <v>414.1935364630534</v>
+        <v>466.5200000015402</v>
       </c>
       <c r="D24" t="n">
-        <v>6474.778370142047</v>
+        <v>7097.599999974625</v>
       </c>
     </row>
     <row r="25">
@@ -782,13 +782,13 @@
         <v>0.7666666666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>12635.33807925911</v>
+        <v>10234.00000000109</v>
       </c>
       <c r="C25" t="n">
-        <v>427.5927052356462</v>
+        <v>489.9599999979274</v>
       </c>
       <c r="D25" t="n">
-        <v>6482.587705592893</v>
+        <v>7165.579999947106</v>
       </c>
     </row>
     <row r="26">
@@ -796,13 +796,13 @@
         <v>0.8</v>
       </c>
       <c r="B26" t="n">
-        <v>12782.60586740629</v>
+        <v>10403.49000000138</v>
       </c>
       <c r="C26" t="n">
-        <v>435.5577939095213</v>
+        <v>504.0899999975995</v>
       </c>
       <c r="D26" t="n">
-        <v>6451.901730266419</v>
+        <v>7137.80999996567</v>
       </c>
     </row>
     <row r="27">
@@ -810,13 +810,13 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="B27" t="n">
-        <v>12962.66049171196</v>
+        <v>10621.34999999932</v>
       </c>
       <c r="C27" t="n">
-        <v>447.4189084122374</v>
+        <v>515.7499999977515</v>
       </c>
       <c r="D27" t="n">
-        <v>6407.085948404506</v>
+        <v>7128.009999975996</v>
       </c>
     </row>
     <row r="28">
@@ -824,13 +824,13 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="B28" t="n">
-        <v>13083.54188627047</v>
+        <v>10734.14000000031</v>
       </c>
       <c r="C28" t="n">
-        <v>461.2612545024355</v>
+        <v>523.4199999977933</v>
       </c>
       <c r="D28" t="n">
-        <v>6355.752448061746</v>
+        <v>7071.06999997977</v>
       </c>
     </row>
     <row r="29">
@@ -838,13 +838,13 @@
         <v>0.9</v>
       </c>
       <c r="B29" t="n">
-        <v>13266.07278680368</v>
+        <v>10908.66999999769</v>
       </c>
       <c r="C29" t="n">
-        <v>468.3337443280442</v>
+        <v>538.2199999988134</v>
       </c>
       <c r="D29" t="n">
-        <v>6312.354616102235</v>
+        <v>7044.279999981088</v>
       </c>
     </row>
     <row r="30">
@@ -852,13 +852,13 @@
         <v>0.9333333333333333</v>
       </c>
       <c r="B30" t="n">
-        <v>13394.54002793477</v>
+        <v>11092.19000000006</v>
       </c>
       <c r="C30" t="n">
-        <v>478.5028027028271</v>
+        <v>543.8399999975765</v>
       </c>
       <c r="D30" t="n">
-        <v>6257.337492328858</v>
+        <v>7003.649999986912</v>
       </c>
     </row>
     <row r="31">
@@ -866,13 +866,13 @@
         <v>0.9666666666666667</v>
       </c>
       <c r="B31" t="n">
-        <v>13518.25868908472</v>
+        <v>11159.10999999905</v>
       </c>
       <c r="C31" t="n">
-        <v>485.0739095759201</v>
+        <v>544.749999994508</v>
       </c>
       <c r="D31" t="n">
-        <v>6147.866861531261</v>
+        <v>6882.629999988557</v>
       </c>
     </row>
     <row r="32">
@@ -880,13 +880,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>13803.21419372251</v>
+        <v>11235.19000000273</v>
       </c>
       <c r="C32" t="n">
-        <v>459.04321535677</v>
+        <v>555.5199999975032</v>
       </c>
       <c r="D32" t="n">
-        <v>6122.895502285376</v>
+        <v>6781.669999990558</v>
       </c>
     </row>
     <row r="33">
@@ -894,13 +894,13 @@
         <v>1.033333333333333</v>
       </c>
       <c r="B33" t="n">
-        <v>13952.14365383609</v>
+        <v>11479.58999999977</v>
       </c>
       <c r="C33" t="n">
-        <v>467.1473963087757</v>
+        <v>568.4399999981766</v>
       </c>
       <c r="D33" t="n">
-        <v>6049.27606144307</v>
+        <v>6753.159999991508</v>
       </c>
     </row>
     <row r="34">
@@ -908,13 +908,13 @@
         <v>1.066666666666667</v>
       </c>
       <c r="B34" t="n">
-        <v>14030.55613453701</v>
+        <v>11613.32999999987</v>
       </c>
       <c r="C34" t="n">
-        <v>485.350364637565</v>
+        <v>586.6099999963463</v>
       </c>
       <c r="D34" t="n">
-        <v>5966.33096611939</v>
+        <v>6670.659999990923</v>
       </c>
     </row>
     <row r="35">
@@ -922,13 +922,13 @@
         <v>1.1</v>
       </c>
       <c r="B35" t="n">
-        <v>14179.82315872458</v>
+        <v>11764.54000000327</v>
       </c>
       <c r="C35" t="n">
-        <v>505.1371702543942</v>
+        <v>605.3699999955072</v>
       </c>
       <c r="D35" t="n">
-        <v>5906.037691588646</v>
+        <v>6583.619999989382</v>
       </c>
     </row>
     <row r="36">
@@ -936,13 +936,13 @@
         <v>1.133333333333333</v>
       </c>
       <c r="B36" t="n">
-        <v>14394.52610147837</v>
+        <v>11969.87999999765</v>
       </c>
       <c r="C36" t="n">
-        <v>506.8776412173643</v>
+        <v>611.9199999967831</v>
       </c>
       <c r="D36" t="n">
-        <v>5810.189512517667</v>
+        <v>6517.909999991484</v>
       </c>
     </row>
     <row r="37">
@@ -950,13 +950,13 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37" t="n">
-        <v>14503.81357347808</v>
+        <v>12049.89999999633</v>
       </c>
       <c r="C37" t="n">
-        <v>520.8293881374873</v>
+        <v>613.1499999974591</v>
       </c>
       <c r="D37" t="n">
-        <v>5699.648857028375</v>
+        <v>6396.819999992181</v>
       </c>
     </row>
     <row r="38">
@@ -964,13 +964,13 @@
         <v>1.2</v>
       </c>
       <c r="B38" t="n">
-        <v>14649.18554172886</v>
+        <v>12130.57999999643</v>
       </c>
       <c r="C38" t="n">
-        <v>528.5191406727265</v>
+        <v>624.2700000025008</v>
       </c>
       <c r="D38" t="n">
-        <v>5601.15213057723</v>
+        <v>6270.549999993863</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         <v>1.233333333333333</v>
       </c>
       <c r="B39" t="n">
-        <v>14776.55981597375</v>
+        <v>12359.99000000052</v>
       </c>
       <c r="C39" t="n">
-        <v>540.6026932258874</v>
+        <v>651.5099999980665</v>
       </c>
       <c r="D39" t="n">
-        <v>5500.676729919274</v>
+        <v>6186.699999991491</v>
       </c>
     </row>
     <row r="40">
@@ -992,13 +992,13 @@
         <v>1.266666666666667</v>
       </c>
       <c r="B40" t="n">
-        <v>14946.05459987146</v>
+        <v>12588.01999999735</v>
       </c>
       <c r="C40" t="n">
-        <v>554.2200523336803</v>
+        <v>669.1499999948815</v>
       </c>
       <c r="D40" t="n">
-        <v>5388.849305042385</v>
+        <v>6114.609999994512</v>
       </c>
     </row>
     <row r="41">
@@ -1006,13 +1006,13 @@
         <v>1.3</v>
       </c>
       <c r="B41" t="n">
-        <v>15022.46331036672</v>
+        <v>12602.5599999957</v>
       </c>
       <c r="C41" t="n">
-        <v>589.6639227267999</v>
+        <v>672.2899999989572</v>
       </c>
       <c r="D41" t="n">
-        <v>5231.684012435935</v>
+        <v>5944.189999993511</v>
       </c>
     </row>
     <row r="42">
@@ -1020,13 +1020,13 @@
         <v>1.333333333333333</v>
       </c>
       <c r="B42" t="n">
-        <v>15150.20247258959</v>
+        <v>12707.61999999675</v>
       </c>
       <c r="C42" t="n">
-        <v>599.6217302859592</v>
+        <v>674.1499999963195</v>
       </c>
       <c r="D42" t="n">
-        <v>5105.566710040019</v>
+        <v>5807.61999999308</v>
       </c>
     </row>
     <row r="43">
@@ -1034,13 +1034,13 @@
         <v>1.366666666666667</v>
       </c>
       <c r="B43" t="n">
-        <v>15251.533915885</v>
+        <v>12739.23999999427</v>
       </c>
       <c r="C43" t="n">
-        <v>607.6474737616869</v>
+        <v>687.8499999930369</v>
       </c>
       <c r="D43" t="n">
-        <v>4967.486267451978</v>
+        <v>5640.059999997088</v>
       </c>
     </row>
     <row r="44">
@@ -1048,13 +1048,13 @@
         <v>1.4</v>
       </c>
       <c r="B44" t="n">
-        <v>15353.17079266563</v>
+        <v>12832.78999999597</v>
       </c>
       <c r="C44" t="n">
-        <v>606.7788020492254</v>
+        <v>689.2899999943718</v>
       </c>
       <c r="D44" t="n">
-        <v>4824.690910951283</v>
+        <v>5494.319999995717</v>
       </c>
     </row>
     <row r="45">
@@ -1062,13 +1062,13 @@
         <v>1.433333333333333</v>
       </c>
       <c r="B45" t="n">
-        <v>15495.65087828405</v>
+        <v>13008.69999999173</v>
       </c>
       <c r="C45" t="n">
-        <v>617.3690200466482</v>
+        <v>709.4299999928879</v>
       </c>
       <c r="D45" t="n">
-        <v>4674.281689593379</v>
+        <v>5369.499999994586</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>1.466666666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>15547.2376000273</v>
+        <v>13115.37999998869</v>
       </c>
       <c r="C46" t="n">
-        <v>626.1883589175171</v>
+        <v>721.1799999967396</v>
       </c>
       <c r="D46" t="n">
-        <v>4712.605034101749</v>
+        <v>5200.52999999441</v>
       </c>
     </row>
     <row r="47">
@@ -1090,13 +1090,13 @@
         <v>1.5</v>
       </c>
       <c r="B47" t="n">
-        <v>15724.50491018924</v>
+        <v>13150.98999999522</v>
       </c>
       <c r="C47" t="n">
-        <v>639.3888747846812</v>
+        <v>724.7999999955713</v>
       </c>
       <c r="D47" t="n">
-        <v>4564.993103103866</v>
+        <v>5031.069999993471</v>
       </c>
     </row>
     <row r="48">
@@ -1104,13 +1104,13 @@
         <v>1.533333333333333</v>
       </c>
       <c r="B48" t="n">
-        <v>15825.63908986542</v>
+        <v>13395.45999998197</v>
       </c>
       <c r="C48" t="n">
-        <v>653.7152853326515</v>
+        <v>743.3099999950385</v>
       </c>
       <c r="D48" t="n">
-        <v>4359.242939525529</v>
+        <v>4921.509999999733</v>
       </c>
     </row>
     <row r="49">
@@ -1118,13 +1118,13 @@
         <v>1.566666666666667</v>
       </c>
       <c r="B49" t="n">
-        <v>15816.64570403627</v>
+        <v>13370.26999999225</v>
       </c>
       <c r="C49" t="n">
-        <v>658.9732495405109</v>
+        <v>748.7999999896318</v>
       </c>
       <c r="D49" t="n">
-        <v>4219.808790577632</v>
+        <v>4720.519999999476</v>
       </c>
     </row>
     <row r="50">
@@ -1132,13 +1132,13 @@
         <v>1.6</v>
       </c>
       <c r="B50" t="n">
-        <v>15882.40260383775</v>
+        <v>13333.14000000043</v>
       </c>
       <c r="C50" t="n">
-        <v>663.03957339252</v>
+        <v>743.880000002035</v>
       </c>
       <c r="D50" t="n">
-        <v>4042.576813177311</v>
+        <v>4534.58000000141</v>
       </c>
     </row>
     <row r="51">
@@ -1146,13 +1146,13 @@
         <v>1.633333333333333</v>
       </c>
       <c r="B51" t="n">
-        <v>15991.98449512698</v>
+        <v>13445.13999999474</v>
       </c>
       <c r="C51" t="n">
-        <v>680.0236443376853</v>
+        <v>755.8299999987887</v>
       </c>
       <c r="D51" t="n">
-        <v>3884.867874989115</v>
+        <v>4373.049999997904</v>
       </c>
     </row>
     <row r="52">
@@ -1160,13 +1160,13 @@
         <v>1.666666666666667</v>
       </c>
       <c r="B52" t="n">
-        <v>16038.87273219378</v>
+        <v>13551.29999999237</v>
       </c>
       <c r="C52" t="n">
-        <v>684.1602477308907</v>
+        <v>767.4399999974082</v>
       </c>
       <c r="D52" t="n">
-        <v>3694.313656268508</v>
+        <v>4199.790000001665</v>
       </c>
     </row>
     <row r="53">
@@ -1174,13 +1174,13 @@
         <v>1.7</v>
       </c>
       <c r="B53" t="n">
-        <v>16146.87503836606</v>
+        <v>13608.52999998706</v>
       </c>
       <c r="C53" t="n">
-        <v>688.6961366589838</v>
+        <v>771.2599999963095</v>
       </c>
       <c r="D53" t="n">
-        <v>3521.044733130797</v>
+        <v>4001.119999999608</v>
       </c>
     </row>
     <row r="54">
@@ -1188,13 +1188,13 @@
         <v>1.733333333333333</v>
       </c>
       <c r="B54" t="n">
-        <v>16171.25157442826</v>
+        <v>13726.71999998878</v>
       </c>
       <c r="C54" t="n">
-        <v>697.844832067479</v>
+        <v>783.4699999957804</v>
       </c>
       <c r="D54" t="n">
-        <v>3353.597435200341</v>
+        <v>3840.499999999764</v>
       </c>
     </row>
     <row r="55">
@@ -1202,13 +1202,13 @@
         <v>1.766666666666667</v>
       </c>
       <c r="B55" t="n">
-        <v>16326.80931032308</v>
+        <v>13918.67999997712</v>
       </c>
       <c r="C55" t="n">
-        <v>710.5484596831826</v>
+        <v>794.05999999166</v>
       </c>
       <c r="D55" t="n">
-        <v>3241.326560632477</v>
+        <v>3678.789999997231</v>
       </c>
     </row>
     <row r="56">
@@ -1216,13 +1216,13 @@
         <v>1.8</v>
       </c>
       <c r="B56" t="n">
-        <v>16292.45509438363</v>
+        <v>13742.87999999287</v>
       </c>
       <c r="C56" t="n">
-        <v>703.7043182293438</v>
+        <v>781.8199999985792</v>
       </c>
       <c r="D56" t="n">
-        <v>3028.170349030047</v>
+        <v>3454.109999999766</v>
       </c>
     </row>
     <row r="57">
@@ -1230,13 +1230,13 @@
         <v>1.833333333333333</v>
       </c>
       <c r="B57" t="n">
-        <v>16391.6557173154</v>
+        <v>13944.9999999824</v>
       </c>
       <c r="C57" t="n">
-        <v>719.6538677611444</v>
+        <v>802.4799999931125</v>
       </c>
       <c r="D57" t="n">
-        <v>2851.684331980192</v>
+        <v>3275.180000007429</v>
       </c>
     </row>
     <row r="58">
@@ -1244,13 +1244,13 @@
         <v>1.866666666666667</v>
       </c>
       <c r="B58" t="n">
-        <v>16310.10330524439</v>
+        <v>13988.45999997337</v>
       </c>
       <c r="C58" t="n">
-        <v>720.8222740452042</v>
+        <v>805.7099999845256</v>
       </c>
       <c r="D58" t="n">
-        <v>2725.444665999593</v>
+        <v>3083.880000006923</v>
       </c>
     </row>
     <row r="59">
@@ -1258,13 +1258,13 @@
         <v>1.9</v>
       </c>
       <c r="B59" t="n">
-        <v>16328.71322415624</v>
+        <v>13970.2299999893</v>
       </c>
       <c r="C59" t="n">
-        <v>719.7241746379351</v>
+        <v>800.9499999959012</v>
       </c>
       <c r="D59" t="n">
-        <v>2589.574228227048</v>
+        <v>2890.300000010958</v>
       </c>
     </row>
     <row r="60">
@@ -1272,13 +1272,13 @@
         <v>1.933333333333333</v>
       </c>
       <c r="B60" t="n">
-        <v>16491.15666107844</v>
+        <v>14025.54999997833</v>
       </c>
       <c r="C60" t="n">
-        <v>727.074726067095</v>
+        <v>814.3699999850752</v>
       </c>
       <c r="D60" t="n">
-        <v>2469.21720801251</v>
+        <v>2695.140000009903</v>
       </c>
     </row>
     <row r="61">
@@ -1286,13 +1286,13 @@
         <v>1.966666666666667</v>
       </c>
       <c r="B61" t="n">
-        <v>16498.49445850071</v>
+        <v>14078.76999997624</v>
       </c>
       <c r="C61" t="n">
-        <v>725.6516637540846</v>
+        <v>807.7899999927205</v>
       </c>
       <c r="D61" t="n">
-        <v>2381.329938304832</v>
+        <v>2487.400000016846</v>
       </c>
     </row>
     <row r="62">
@@ -1300,13 +1300,13 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>16517.7241203987</v>
+        <v>14218.23999996147</v>
       </c>
       <c r="C62" t="n">
-        <v>728.3680258620219</v>
+        <v>820.3499999898225</v>
       </c>
       <c r="D62" t="n">
-        <v>2303.552214656896</v>
+        <v>2303.57000002623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
successfully implemented time-series based XGB regression but needs tidying up and optimization
</commit_message>
<xml_diff>
--- a/VisionModel/one_model/output/predicted_trajectoriesCombined.xlsx
+++ b/VisionModel/one_model/output/predicted_trajectoriesCombined.xlsx
@@ -460,13 +460,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1571.110000049326</v>
+        <v>4042.261178533166</v>
       </c>
       <c r="C2" t="n">
-        <v>274.5400000030443</v>
+        <v>99.63138986942523</v>
       </c>
       <c r="D2" t="n">
-        <v>2788.830000029995</v>
+        <v>2872.758718594442</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>0.03333333333333333</v>
       </c>
       <c r="B3" t="n">
-        <v>2383.240000027599</v>
+        <v>4843.104700189625</v>
       </c>
       <c r="C3" t="n">
-        <v>297.3199999984293</v>
+        <v>133.684749483326</v>
       </c>
       <c r="D3" t="n">
-        <v>3318.210000016494</v>
+        <v>3335.020037985748</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>0.06666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>3167.01000002484</v>
+        <v>5694.049009783843</v>
       </c>
       <c r="C4" t="n">
-        <v>292.0400000030752</v>
+        <v>132.0249906400697</v>
       </c>
       <c r="D4" t="n">
-        <v>3856.950000006812</v>
+        <v>3798.162259809709</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>3929.380000025288</v>
+        <v>6438.611309263215</v>
       </c>
       <c r="C5" t="n">
-        <v>292.4500000063812</v>
+        <v>146.4752784414153</v>
       </c>
       <c r="D5" t="n">
-        <v>4345.590000004549</v>
+        <v>4245.31533836317</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="B6" t="n">
-        <v>4505.530000018184</v>
+        <v>7059.882565624657</v>
       </c>
       <c r="C6" t="n">
-        <v>311.4300000009518</v>
+        <v>163.6983367069226</v>
       </c>
       <c r="D6" t="n">
-        <v>4718.390000000028</v>
+        <v>4600.02708193398</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="B7" t="n">
-        <v>4997.76000001644</v>
+        <v>7603.291433288357</v>
       </c>
       <c r="C7" t="n">
-        <v>312.0700000017562</v>
+        <v>173.9658407765299</v>
       </c>
       <c r="D7" t="n">
-        <v>5030.869999999372</v>
+        <v>4833.91336467765</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>5410.030000016259</v>
+        <v>8032.262111407125</v>
       </c>
       <c r="C8" t="n">
-        <v>331.6100000020058</v>
+        <v>190.6088938661355</v>
       </c>
       <c r="D8" t="n">
-        <v>5275.739999995401</v>
+        <v>5058.054074345984</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>0.2333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>5845.5200000103</v>
+        <v>8313.879475221485</v>
       </c>
       <c r="C9" t="n">
-        <v>343.7600000025757</v>
+        <v>199.6609295146157</v>
       </c>
       <c r="D9" t="n">
-        <v>5553.899999997995</v>
+        <v>5296.037405313211</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="B10" t="n">
-        <v>6268.930000013829</v>
+        <v>8729.470243753516</v>
       </c>
       <c r="C10" t="n">
-        <v>347.7900000005106</v>
+        <v>212.6384564337307</v>
       </c>
       <c r="D10" t="n">
-        <v>5778.159999993276</v>
+        <v>5451.621370691195</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>0.3</v>
       </c>
       <c r="B11" t="n">
-        <v>6685.410000010121</v>
+        <v>9112.563602116979</v>
       </c>
       <c r="C11" t="n">
-        <v>354.2300000000048</v>
+        <v>238.6504178826896</v>
       </c>
       <c r="D11" t="n">
-        <v>6036.049999996207</v>
+        <v>5629.086028057161</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="B12" t="n">
-        <v>6968.70000000934</v>
+        <v>9453.505841529721</v>
       </c>
       <c r="C12" t="n">
-        <v>357.7699999983905</v>
+        <v>243.6519269973406</v>
       </c>
       <c r="D12" t="n">
-        <v>6182.399999994025</v>
+        <v>5764.157092739942</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>0.3666666666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>7315.880000013184</v>
+        <v>9774.924001650776</v>
       </c>
       <c r="C13" t="n">
-        <v>373.4699999995082</v>
+        <v>258.6806115824122</v>
       </c>
       <c r="D13" t="n">
-        <v>6337.779999992428</v>
+        <v>5898.040155849277</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +628,13 @@
         <v>0.4</v>
       </c>
       <c r="B14" t="n">
-        <v>7642.340000007943</v>
+        <v>10177.41970499595</v>
       </c>
       <c r="C14" t="n">
-        <v>385.2800000009273</v>
+        <v>277.3238092996165</v>
       </c>
       <c r="D14" t="n">
-        <v>6505.66999999364</v>
+        <v>6027.284754104194</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +642,13 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="B15" t="n">
-        <v>7942.840000003797</v>
+        <v>10457.61164861421</v>
       </c>
       <c r="C15" t="n">
-        <v>395.6700000015693</v>
+        <v>285.959734488659</v>
       </c>
       <c r="D15" t="n">
-        <v>6623.369999998818</v>
+        <v>6129.933177734317</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +656,13 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="B16" t="n">
-        <v>8211.29000000339</v>
+        <v>10739.56104438033</v>
       </c>
       <c r="C16" t="n">
-        <v>401.2499999987305</v>
+        <v>331.8596349857691</v>
       </c>
       <c r="D16" t="n">
-        <v>6731.089999994469</v>
+        <v>6242.907871355815</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +670,13 @@
         <v>0.5</v>
       </c>
       <c r="B17" t="n">
-        <v>8421.110000003007</v>
+        <v>10991.37258145039</v>
       </c>
       <c r="C17" t="n">
-        <v>412.3299999969155</v>
+        <v>341.3306269331836</v>
       </c>
       <c r="D17" t="n">
-        <v>6804.669999988783</v>
+        <v>6313.858401919963</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +684,13 @@
         <v>0.5333333333333333</v>
       </c>
       <c r="B18" t="n">
-        <v>8687.100000003398</v>
+        <v>11177.68563349658</v>
       </c>
       <c r="C18" t="n">
-        <v>413.3100000000913</v>
+        <v>347.8315910842927</v>
       </c>
       <c r="D18" t="n">
-        <v>6891.139999989607</v>
+        <v>6338.408447373296</v>
       </c>
     </row>
     <row r="19">
@@ -698,13 +698,13 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>8971.030000005254</v>
+        <v>11417.61049189586</v>
       </c>
       <c r="C19" t="n">
-        <v>439.259999998176</v>
+        <v>367.4942650344049</v>
       </c>
       <c r="D19" t="n">
-        <v>6975.359999986497</v>
+        <v>6366.887305438978</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +712,13 @@
         <v>0.6</v>
       </c>
       <c r="B20" t="n">
-        <v>9256.210000000277</v>
+        <v>11595.06932656615</v>
       </c>
       <c r="C20" t="n">
-        <v>457.7999999929814</v>
+        <v>381.6807619050949</v>
       </c>
       <c r="D20" t="n">
-        <v>7071.049999983691</v>
+        <v>6446.558841296247</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +726,13 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>9430.740000004758</v>
+        <v>11777.512002425</v>
       </c>
       <c r="C21" t="n">
-        <v>450.6400000024637</v>
+        <v>384.4399606484644</v>
       </c>
       <c r="D21" t="n">
-        <v>7093.659999957395</v>
+        <v>6463.165291660873</v>
       </c>
     </row>
     <row r="22">
@@ -740,13 +740,13 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>9565.119999998285</v>
+        <v>11997.33539222781</v>
       </c>
       <c r="C22" t="n">
-        <v>454.6500000005836</v>
+        <v>391.6039521416105</v>
       </c>
       <c r="D22" t="n">
-        <v>7081.369999981678</v>
+        <v>6489.928969743357</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>0.7</v>
       </c>
       <c r="B23" t="n">
-        <v>9660.709999993989</v>
+        <v>12128.77514305258</v>
       </c>
       <c r="C23" t="n">
-        <v>461.4300000003938</v>
+        <v>398.3599774891508</v>
       </c>
       <c r="D23" t="n">
-        <v>7030.679999993657</v>
+        <v>6449.104745751848</v>
       </c>
     </row>
     <row r="24">
@@ -768,13 +768,13 @@
         <v>0.7333333333333333</v>
       </c>
       <c r="B24" t="n">
-        <v>9942.999999999667</v>
+        <v>12392.78709634662</v>
       </c>
       <c r="C24" t="n">
-        <v>466.5200000015402</v>
+        <v>414.1935364630534</v>
       </c>
       <c r="D24" t="n">
-        <v>7097.599999974625</v>
+        <v>6474.778370142047</v>
       </c>
     </row>
     <row r="25">
@@ -782,13 +782,13 @@
         <v>0.7666666666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>10234.00000000109</v>
+        <v>12635.33807925911</v>
       </c>
       <c r="C25" t="n">
-        <v>489.9599999979274</v>
+        <v>427.5927052356462</v>
       </c>
       <c r="D25" t="n">
-        <v>7165.579999947106</v>
+        <v>6482.587705592893</v>
       </c>
     </row>
     <row r="26">
@@ -796,13 +796,13 @@
         <v>0.8</v>
       </c>
       <c r="B26" t="n">
-        <v>10403.49000000138</v>
+        <v>12782.60586740629</v>
       </c>
       <c r="C26" t="n">
-        <v>504.0899999975995</v>
+        <v>435.5577939095213</v>
       </c>
       <c r="D26" t="n">
-        <v>7137.80999996567</v>
+        <v>6451.901730266419</v>
       </c>
     </row>
     <row r="27">
@@ -810,13 +810,13 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="B27" t="n">
-        <v>10621.34999999932</v>
+        <v>12962.66049171196</v>
       </c>
       <c r="C27" t="n">
-        <v>515.7499999977515</v>
+        <v>447.4189084122374</v>
       </c>
       <c r="D27" t="n">
-        <v>7128.009999975996</v>
+        <v>6407.085948404506</v>
       </c>
     </row>
     <row r="28">
@@ -824,13 +824,13 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="B28" t="n">
-        <v>10734.14000000031</v>
+        <v>13083.54188627047</v>
       </c>
       <c r="C28" t="n">
-        <v>523.4199999977933</v>
+        <v>461.2612545024355</v>
       </c>
       <c r="D28" t="n">
-        <v>7071.06999997977</v>
+        <v>6355.752448061746</v>
       </c>
     </row>
     <row r="29">
@@ -838,13 +838,13 @@
         <v>0.9</v>
       </c>
       <c r="B29" t="n">
-        <v>10908.66999999769</v>
+        <v>13266.07278680368</v>
       </c>
       <c r="C29" t="n">
-        <v>538.2199999988134</v>
+        <v>468.3337443280442</v>
       </c>
       <c r="D29" t="n">
-        <v>7044.279999981088</v>
+        <v>6312.354616102235</v>
       </c>
     </row>
     <row r="30">
@@ -852,13 +852,13 @@
         <v>0.9333333333333333</v>
       </c>
       <c r="B30" t="n">
-        <v>11092.19000000006</v>
+        <v>13394.54002793477</v>
       </c>
       <c r="C30" t="n">
-        <v>543.8399999975765</v>
+        <v>478.5028027028271</v>
       </c>
       <c r="D30" t="n">
-        <v>7003.649999986912</v>
+        <v>6257.337492328858</v>
       </c>
     </row>
     <row r="31">
@@ -866,13 +866,13 @@
         <v>0.9666666666666667</v>
       </c>
       <c r="B31" t="n">
-        <v>11159.10999999905</v>
+        <v>13518.25868908472</v>
       </c>
       <c r="C31" t="n">
-        <v>544.749999994508</v>
+        <v>485.0739095759201</v>
       </c>
       <c r="D31" t="n">
-        <v>6882.629999988557</v>
+        <v>6147.866861531261</v>
       </c>
     </row>
     <row r="32">
@@ -880,13 +880,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>11235.19000000273</v>
+        <v>13803.21419372251</v>
       </c>
       <c r="C32" t="n">
-        <v>555.5199999975032</v>
+        <v>459.04321535677</v>
       </c>
       <c r="D32" t="n">
-        <v>6781.669999990558</v>
+        <v>6122.895502285376</v>
       </c>
     </row>
     <row r="33">
@@ -894,13 +894,13 @@
         <v>1.033333333333333</v>
       </c>
       <c r="B33" t="n">
-        <v>11479.58999999977</v>
+        <v>13952.14365383609</v>
       </c>
       <c r="C33" t="n">
-        <v>568.4399999981766</v>
+        <v>467.1473963087757</v>
       </c>
       <c r="D33" t="n">
-        <v>6753.159999991508</v>
+        <v>6049.27606144307</v>
       </c>
     </row>
     <row r="34">
@@ -908,13 +908,13 @@
         <v>1.066666666666667</v>
       </c>
       <c r="B34" t="n">
-        <v>11613.32999999987</v>
+        <v>14030.55613453701</v>
       </c>
       <c r="C34" t="n">
-        <v>586.6099999963463</v>
+        <v>485.350364637565</v>
       </c>
       <c r="D34" t="n">
-        <v>6670.659999990923</v>
+        <v>5966.33096611939</v>
       </c>
     </row>
     <row r="35">
@@ -922,13 +922,13 @@
         <v>1.1</v>
       </c>
       <c r="B35" t="n">
-        <v>11764.54000000327</v>
+        <v>14179.82315872458</v>
       </c>
       <c r="C35" t="n">
-        <v>605.3699999955072</v>
+        <v>505.1371702543942</v>
       </c>
       <c r="D35" t="n">
-        <v>6583.619999989382</v>
+        <v>5906.037691588646</v>
       </c>
     </row>
     <row r="36">
@@ -936,13 +936,13 @@
         <v>1.133333333333333</v>
       </c>
       <c r="B36" t="n">
-        <v>11969.87999999765</v>
+        <v>14394.52610147837</v>
       </c>
       <c r="C36" t="n">
-        <v>611.9199999967831</v>
+        <v>506.8776412173643</v>
       </c>
       <c r="D36" t="n">
-        <v>6517.909999991484</v>
+        <v>5810.189512517667</v>
       </c>
     </row>
     <row r="37">
@@ -950,13 +950,13 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37" t="n">
-        <v>12049.89999999633</v>
+        <v>14503.81357347808</v>
       </c>
       <c r="C37" t="n">
-        <v>613.1499999974591</v>
+        <v>520.8293881374873</v>
       </c>
       <c r="D37" t="n">
-        <v>6396.819999992181</v>
+        <v>5699.648857028375</v>
       </c>
     </row>
     <row r="38">
@@ -964,13 +964,13 @@
         <v>1.2</v>
       </c>
       <c r="B38" t="n">
-        <v>12130.57999999643</v>
+        <v>14649.18554172886</v>
       </c>
       <c r="C38" t="n">
-        <v>624.2700000025008</v>
+        <v>528.5191406727265</v>
       </c>
       <c r="D38" t="n">
-        <v>6270.549999993863</v>
+        <v>5601.15213057723</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         <v>1.233333333333333</v>
       </c>
       <c r="B39" t="n">
-        <v>12359.99000000052</v>
+        <v>14776.55981597375</v>
       </c>
       <c r="C39" t="n">
-        <v>651.5099999980665</v>
+        <v>540.6026932258874</v>
       </c>
       <c r="D39" t="n">
-        <v>6186.699999991491</v>
+        <v>5500.676729919274</v>
       </c>
     </row>
     <row r="40">
@@ -992,13 +992,13 @@
         <v>1.266666666666667</v>
       </c>
       <c r="B40" t="n">
-        <v>12588.01999999735</v>
+        <v>14946.05459987146</v>
       </c>
       <c r="C40" t="n">
-        <v>669.1499999948815</v>
+        <v>554.2200523336803</v>
       </c>
       <c r="D40" t="n">
-        <v>6114.609999994512</v>
+        <v>5388.849305042385</v>
       </c>
     </row>
     <row r="41">
@@ -1006,13 +1006,13 @@
         <v>1.3</v>
       </c>
       <c r="B41" t="n">
-        <v>12602.5599999957</v>
+        <v>15022.46331036672</v>
       </c>
       <c r="C41" t="n">
-        <v>672.2899999989572</v>
+        <v>589.6639227267999</v>
       </c>
       <c r="D41" t="n">
-        <v>5944.189999993511</v>
+        <v>5231.684012435935</v>
       </c>
     </row>
     <row r="42">
@@ -1020,13 +1020,13 @@
         <v>1.333333333333333</v>
       </c>
       <c r="B42" t="n">
-        <v>12707.61999999675</v>
+        <v>15150.20247258959</v>
       </c>
       <c r="C42" t="n">
-        <v>674.1499999963195</v>
+        <v>599.6217302859592</v>
       </c>
       <c r="D42" t="n">
-        <v>5807.61999999308</v>
+        <v>5105.566710040019</v>
       </c>
     </row>
     <row r="43">
@@ -1034,13 +1034,13 @@
         <v>1.366666666666667</v>
       </c>
       <c r="B43" t="n">
-        <v>12739.23999999427</v>
+        <v>15251.533915885</v>
       </c>
       <c r="C43" t="n">
-        <v>687.8499999930369</v>
+        <v>607.6474737616869</v>
       </c>
       <c r="D43" t="n">
-        <v>5640.059999997088</v>
+        <v>4967.486267451978</v>
       </c>
     </row>
     <row r="44">
@@ -1048,13 +1048,13 @@
         <v>1.4</v>
       </c>
       <c r="B44" t="n">
-        <v>12832.78999999597</v>
+        <v>15353.17079266563</v>
       </c>
       <c r="C44" t="n">
-        <v>689.2899999943718</v>
+        <v>606.7788020492254</v>
       </c>
       <c r="D44" t="n">
-        <v>5494.319999995717</v>
+        <v>4824.690910951283</v>
       </c>
     </row>
     <row r="45">
@@ -1062,13 +1062,13 @@
         <v>1.433333333333333</v>
       </c>
       <c r="B45" t="n">
-        <v>13008.69999999173</v>
+        <v>15495.65087828405</v>
       </c>
       <c r="C45" t="n">
-        <v>709.4299999928879</v>
+        <v>617.3690200466482</v>
       </c>
       <c r="D45" t="n">
-        <v>5369.499999994586</v>
+        <v>4674.281689593379</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>1.466666666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>13115.37999998869</v>
+        <v>15547.2376000273</v>
       </c>
       <c r="C46" t="n">
-        <v>721.1799999967396</v>
+        <v>626.1883589175171</v>
       </c>
       <c r="D46" t="n">
-        <v>5200.52999999441</v>
+        <v>4712.605034101749</v>
       </c>
     </row>
     <row r="47">
@@ -1090,13 +1090,13 @@
         <v>1.5</v>
       </c>
       <c r="B47" t="n">
-        <v>13150.98999999522</v>
+        <v>15724.50491018924</v>
       </c>
       <c r="C47" t="n">
-        <v>724.7999999955713</v>
+        <v>639.3888747846812</v>
       </c>
       <c r="D47" t="n">
-        <v>5031.069999993471</v>
+        <v>4564.993103103866</v>
       </c>
     </row>
     <row r="48">
@@ -1104,13 +1104,13 @@
         <v>1.533333333333333</v>
       </c>
       <c r="B48" t="n">
-        <v>13395.45999998197</v>
+        <v>15825.63908986542</v>
       </c>
       <c r="C48" t="n">
-        <v>743.3099999950385</v>
+        <v>653.7152853326515</v>
       </c>
       <c r="D48" t="n">
-        <v>4921.509999999733</v>
+        <v>4359.242939525529</v>
       </c>
     </row>
     <row r="49">
@@ -1118,13 +1118,13 @@
         <v>1.566666666666667</v>
       </c>
       <c r="B49" t="n">
-        <v>13370.26999999225</v>
+        <v>15816.64570403627</v>
       </c>
       <c r="C49" t="n">
-        <v>748.7999999896318</v>
+        <v>658.9732495405109</v>
       </c>
       <c r="D49" t="n">
-        <v>4720.519999999476</v>
+        <v>4219.808790577632</v>
       </c>
     </row>
     <row r="50">
@@ -1132,13 +1132,13 @@
         <v>1.6</v>
       </c>
       <c r="B50" t="n">
-        <v>13333.14000000043</v>
+        <v>15882.40260383775</v>
       </c>
       <c r="C50" t="n">
-        <v>743.880000002035</v>
+        <v>663.03957339252</v>
       </c>
       <c r="D50" t="n">
-        <v>4534.58000000141</v>
+        <v>4042.576813177311</v>
       </c>
     </row>
     <row r="51">
@@ -1146,13 +1146,13 @@
         <v>1.633333333333333</v>
       </c>
       <c r="B51" t="n">
-        <v>13445.13999999474</v>
+        <v>15991.98449512698</v>
       </c>
       <c r="C51" t="n">
-        <v>755.8299999987887</v>
+        <v>680.0236443376853</v>
       </c>
       <c r="D51" t="n">
-        <v>4373.049999997904</v>
+        <v>3884.867874989115</v>
       </c>
     </row>
     <row r="52">
@@ -1160,13 +1160,13 @@
         <v>1.666666666666667</v>
       </c>
       <c r="B52" t="n">
-        <v>13551.29999999237</v>
+        <v>16038.87273219378</v>
       </c>
       <c r="C52" t="n">
-        <v>767.4399999974082</v>
+        <v>684.1602477308907</v>
       </c>
       <c r="D52" t="n">
-        <v>4199.790000001665</v>
+        <v>3694.313656268508</v>
       </c>
     </row>
     <row r="53">
@@ -1174,13 +1174,13 @@
         <v>1.7</v>
       </c>
       <c r="B53" t="n">
-        <v>13608.52999998706</v>
+        <v>16146.87503836606</v>
       </c>
       <c r="C53" t="n">
-        <v>771.2599999963095</v>
+        <v>688.6961366589838</v>
       </c>
       <c r="D53" t="n">
-        <v>4001.119999999608</v>
+        <v>3521.044733130797</v>
       </c>
     </row>
     <row r="54">
@@ -1188,13 +1188,13 @@
         <v>1.733333333333333</v>
       </c>
       <c r="B54" t="n">
-        <v>13726.71999998878</v>
+        <v>16171.25157442826</v>
       </c>
       <c r="C54" t="n">
-        <v>783.4699999957804</v>
+        <v>697.844832067479</v>
       </c>
       <c r="D54" t="n">
-        <v>3840.499999999764</v>
+        <v>3353.597435200341</v>
       </c>
     </row>
     <row r="55">
@@ -1202,13 +1202,13 @@
         <v>1.766666666666667</v>
       </c>
       <c r="B55" t="n">
-        <v>13918.67999997712</v>
+        <v>16326.80931032308</v>
       </c>
       <c r="C55" t="n">
-        <v>794.05999999166</v>
+        <v>710.5484596831826</v>
       </c>
       <c r="D55" t="n">
-        <v>3678.789999997231</v>
+        <v>3241.326560632477</v>
       </c>
     </row>
     <row r="56">
@@ -1216,13 +1216,13 @@
         <v>1.8</v>
       </c>
       <c r="B56" t="n">
-        <v>13742.87999999287</v>
+        <v>16292.45509438363</v>
       </c>
       <c r="C56" t="n">
-        <v>781.8199999985792</v>
+        <v>703.7043182293438</v>
       </c>
       <c r="D56" t="n">
-        <v>3454.109999999766</v>
+        <v>3028.170349030047</v>
       </c>
     </row>
     <row r="57">
@@ -1230,13 +1230,13 @@
         <v>1.833333333333333</v>
       </c>
       <c r="B57" t="n">
-        <v>13944.9999999824</v>
+        <v>16391.6557173154</v>
       </c>
       <c r="C57" t="n">
-        <v>802.4799999931125</v>
+        <v>719.6538677611444</v>
       </c>
       <c r="D57" t="n">
-        <v>3275.180000007429</v>
+        <v>2851.684331980192</v>
       </c>
     </row>
     <row r="58">
@@ -1244,13 +1244,13 @@
         <v>1.866666666666667</v>
       </c>
       <c r="B58" t="n">
-        <v>13988.45999997337</v>
+        <v>16310.10330524439</v>
       </c>
       <c r="C58" t="n">
-        <v>805.7099999845256</v>
+        <v>720.8222740452042</v>
       </c>
       <c r="D58" t="n">
-        <v>3083.880000006923</v>
+        <v>2725.444665999593</v>
       </c>
     </row>
     <row r="59">
@@ -1258,13 +1258,13 @@
         <v>1.9</v>
       </c>
       <c r="B59" t="n">
-        <v>13970.2299999893</v>
+        <v>16328.71322415624</v>
       </c>
       <c r="C59" t="n">
-        <v>800.9499999959012</v>
+        <v>719.7241746379351</v>
       </c>
       <c r="D59" t="n">
-        <v>2890.300000010958</v>
+        <v>2589.574228227048</v>
       </c>
     </row>
     <row r="60">
@@ -1272,13 +1272,13 @@
         <v>1.933333333333333</v>
       </c>
       <c r="B60" t="n">
-        <v>14025.54999997833</v>
+        <v>16491.15666107844</v>
       </c>
       <c r="C60" t="n">
-        <v>814.3699999850752</v>
+        <v>727.074726067095</v>
       </c>
       <c r="D60" t="n">
-        <v>2695.140000009903</v>
+        <v>2469.21720801251</v>
       </c>
     </row>
     <row r="61">
@@ -1286,13 +1286,13 @@
         <v>1.966666666666667</v>
       </c>
       <c r="B61" t="n">
-        <v>14078.76999997624</v>
+        <v>16498.49445850071</v>
       </c>
       <c r="C61" t="n">
-        <v>807.7899999927205</v>
+        <v>725.6516637540846</v>
       </c>
       <c r="D61" t="n">
-        <v>2487.400000016846</v>
+        <v>2381.329938304832</v>
       </c>
     </row>
     <row r="62">
@@ -1300,13 +1300,13 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>14218.23999996147</v>
+        <v>16517.7241203987</v>
       </c>
       <c r="C62" t="n">
-        <v>820.3499999898225</v>
+        <v>728.3680258620219</v>
       </c>
       <c r="D62" t="n">
-        <v>2303.57000002623</v>
+        <v>2303.552214656896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>